<commit_message>
Null dates are now allowed
Null dates are now allowed
</commit_message>
<xml_diff>
--- a/eclipse-workspace/test-files/DateTime.xlsx
+++ b/eclipse-workspace/test-files/DateTime.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Irene</t>
-  </si>
-  <si>
-    <t>3/3/1900  16:25:30 PM</t>
   </si>
 </sst>
 </file>
@@ -390,7 +387,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,9 +512,7 @@
       <c r="D7" s="2">
         <v>0.77083333333333304</v>
       </c>
-      <c r="E7" s="3">
-        <v>337</v>
-      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -543,9 +538,7 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
-        <v>62.770833333333336</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="2">
         <v>0.85416666666666696</v>
       </c>
@@ -560,8 +553,8 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
+      <c r="C10" s="1">
+        <v>37714.236111111109</v>
       </c>
       <c r="D10" s="2">
         <v>0.89583333333333404</v>

</xml_diff>